<commit_message>
New PI for PK
</commit_message>
<xml_diff>
--- a/data/Pang_2018.xlsx
+++ b/data/Pang_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b1145ba93b41240/Dokumente/GitHub/CIT-SimBiology-Toolbox/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/migueltenorio/Documents/GitHub/CIT-SimBiology-Toolbox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{BBB5276F-1BEA-6B47-8C0B-E757E805DC09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7420B1EC-7AC4-42E7-8EC2-EF6B8FADAE38}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690749DC-5AF9-5441-BFC0-AD28B9C64AA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{826E9204-57BD-A249-B33E-2188D49D4B28}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{826E9204-57BD-A249-B33E-2188D49D4B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,10 +60,10 @@
     <t>4T1_Pang_0.001_mgkg</t>
   </si>
   <si>
-    <t>Blood.antiPDL1_Iodine[%ID/g]</t>
-  </si>
-  <si>
-    <t>Tumor.antiPDL1_Iodine[%ID/g]</t>
+    <t>Blood.antiPDL1[%ID/g]</t>
+  </si>
+  <si>
+    <t>Tumor.antiPDL1[%ID/g]</t>
   </si>
 </sst>
 </file>
@@ -104,7 +104,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -422,12 +422,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.296875" customWidth="1"/>
+    <col min="2" max="3" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -514,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -543,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>12</v>
       </c>
@@ -572,7 +572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
@@ -601,7 +601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>48</v>
       </c>
@@ -630,7 +630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>72</v>
       </c>

</xml_diff>